<commit_message>
đăng kí (hoàn thành)
</commit_message>
<xml_diff>
--- a/exel/TestcaseSignUp.xlsx
+++ b/exel/TestcaseSignUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NetBeansProjects\KTPM\exel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F877A-CC4F-4C28-81D8-2D26166D49D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF75E45E-00DD-4981-A004-40DE21C9FE7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{306379C0-197B-499D-B62A-2EC254EE46D5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
   <si>
     <t>Username</t>
   </si>
@@ -69,9 +69,6 @@
     <t>user201</t>
   </si>
   <si>
-    <t>user202</t>
-  </si>
-  <si>
     <t>user203</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>pass k đủ kí tự</t>
   </si>
   <si>
-    <t>adfghjkfghjkfgh1234567</t>
-  </si>
-  <si>
     <t>Kiều Oanh1</t>
   </si>
   <si>
@@ -235,6 +229,18 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>qưertyuiopasdfghjklzxcvbnm</t>
+  </si>
+  <si>
+    <t>1234567890123456</t>
+  </si>
+  <si>
+    <t>Kiều Oanh qưertyuiopasdfghjklzxc</t>
+  </si>
+  <si>
+    <t>qwertyuiopasdfghjklzxcvbnmqwertyuiopasdfghjklzxcvbnm@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -613,7 +619,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -648,11 +654,11 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
@@ -660,30 +666,30 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -697,10 +703,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,41 +723,41 @@
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>1234567</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>6</v>
@@ -760,18 +766,18 @@
         <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>1234567</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -780,12 +786,12 @@
         <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>1234567</v>
@@ -797,12 +803,12 @@
         <v>7</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3">
         <v>1234567</v>
@@ -814,15 +820,15 @@
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="3">
         <v>1234567</v>
@@ -834,15 +840,15 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
         <v>1234567</v>
@@ -854,15 +860,15 @@
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3">
         <v>1234567</v>
@@ -874,15 +880,15 @@
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3">
         <v>1234567</v>
@@ -894,12 +900,12 @@
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3">
         <v>1234567</v>
@@ -914,7 +920,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -931,12 +937,12 @@
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3">
         <v>1234567</v>
@@ -951,12 +957,12 @@
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3">
         <v>1234567</v>
@@ -971,12 +977,12 @@
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3">
         <v>1234567</v>
@@ -991,12 +997,12 @@
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3">
         <v>1234567</v>
@@ -1011,12 +1017,12 @@
         <v>7</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3">
         <v>1234567</v>
@@ -1031,12 +1037,12 @@
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3">
         <v>1234567</v>
@@ -1051,12 +1057,12 @@
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3">
         <v>1234567</v>
@@ -1071,12 +1077,12 @@
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="3">
         <v>1234567</v>
@@ -1091,12 +1097,12 @@
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="3">
         <v>1234567</v>
@@ -1111,12 +1117,12 @@
         <v>7</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="3">
         <v>1234567</v>
@@ -1131,12 +1137,12 @@
         <v>7</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="3">
         <v>1234567</v>
@@ -1151,12 +1157,12 @@
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="3">
         <v>1234567</v>
@@ -1171,12 +1177,12 @@
         <v>7</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="3">
         <v>1234567</v>
@@ -1191,12 +1197,12 @@
         <v>7</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="3">
         <v>1234567</v>
@@ -1211,12 +1217,12 @@
         <v>7</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="3">
         <v>1234567</v>
@@ -1231,12 +1237,12 @@
         <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>